<commit_message>
added CLI fire on main module
</commit_message>
<xml_diff>
--- a/outfile/Groupby_analysis.xlsx
+++ b/outfile/Groupby_analysis.xlsx
@@ -14,17 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Groupby Analysis</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>IdTrx</t>
-  </si>
-  <si>
     <t>min</t>
   </si>
   <si>
@@ -37,22 +31,7 @@
     <t>count</t>
   </si>
   <si>
-    <t>Direction</t>
-  </si>
-  <si>
     <t>Market</t>
-  </si>
-  <si>
-    <t>Received</t>
-  </si>
-  <si>
-    <t>Sent</t>
-  </si>
-  <si>
-    <t>Transit</t>
-  </si>
-  <si>
-    <t>on us</t>
   </si>
   <si>
     <t>Domestic</t>
@@ -416,293 +395,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>6</v>
+      <c r="B4">
+        <v>0.01</v>
+      </c>
+      <c r="C4">
+        <v>1809196.172827196</v>
+      </c>
+      <c r="D4">
+        <v>4260893574.95</v>
+      </c>
+      <c r="E4">
+        <v>1702412</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
+      <c r="B5">
         <v>0.01</v>
       </c>
-      <c r="D6">
-        <v>3330885.855269946</v>
-      </c>
-      <c r="E6">
-        <v>4260893574.95</v>
-      </c>
-      <c r="F6">
-        <v>428520</v>
-      </c>
-      <c r="G6">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>1220342.109934192</v>
-      </c>
-      <c r="I6">
-        <v>2283374</v>
-      </c>
-      <c r="J6">
-        <v>428520</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <v>0.01</v>
-      </c>
-      <c r="D7">
-        <v>136635.7004334922</v>
-      </c>
-      <c r="E7">
+      <c r="C5">
+        <v>134575.8595350195</v>
+      </c>
+      <c r="D5">
         <v>999999999</v>
       </c>
-      <c r="F7">
-        <v>301965</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>723563.1839352243</v>
-      </c>
-      <c r="I7">
-        <v>1447336</v>
-      </c>
-      <c r="J7">
-        <v>301965</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>0.01</v>
-      </c>
-      <c r="D8">
-        <v>1335361.022318006</v>
-      </c>
-      <c r="E8">
-        <v>725200000</v>
-      </c>
-      <c r="F8">
-        <v>1089270</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>1312123.762853103</v>
-      </c>
-      <c r="I8">
-        <v>2283379</v>
-      </c>
-      <c r="J8">
-        <v>1089270</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>0.01</v>
-      </c>
-      <c r="D9">
-        <v>126490.9627028991</v>
-      </c>
-      <c r="E9">
-        <v>519389867.72</v>
-      </c>
-      <c r="F9">
-        <v>266303</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>724886.1988449248</v>
-      </c>
-      <c r="I9">
-        <v>1447317</v>
-      </c>
-      <c r="J9">
-        <v>266303</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>573052.6564309726</v>
-      </c>
-      <c r="E10">
-        <v>495780160.16</v>
-      </c>
-      <c r="F10">
-        <v>7736</v>
-      </c>
-      <c r="G10">
-        <v>498</v>
-      </c>
-      <c r="H10">
-        <v>727500.5243019648</v>
-      </c>
-      <c r="I10">
-        <v>1446948</v>
-      </c>
-      <c r="J10">
-        <v>7736</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>0.63</v>
-      </c>
-      <c r="D11">
-        <v>255139.086889519</v>
-      </c>
-      <c r="E11">
-        <v>227809120</v>
-      </c>
-      <c r="F11">
-        <v>12699</v>
-      </c>
-      <c r="G11">
-        <v>310</v>
-      </c>
-      <c r="H11">
-        <v>721406.3949129853</v>
-      </c>
-      <c r="I11">
-        <v>1447305</v>
-      </c>
-      <c r="J11">
-        <v>12699</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>0.01</v>
-      </c>
-      <c r="D12">
-        <v>1094740.296828253</v>
-      </c>
-      <c r="E12">
-        <v>973065119.13</v>
-      </c>
-      <c r="F12">
-        <v>176886</v>
-      </c>
-      <c r="G12">
-        <v>6</v>
-      </c>
-      <c r="H12">
-        <v>1291191.548709338</v>
-      </c>
-      <c r="I12">
-        <v>2283371</v>
-      </c>
-      <c r="J12">
-        <v>176886</v>
+      <c r="E5">
+        <v>580967</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>